<commit_message>
Preparation publi 210-ballot 7af0ddc1faef0b0e22d781cbd835938a36cae101
</commit_message>
<xml_diff>
--- a/387-preparation-release-210-ballot/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
+++ b/387-preparation-release-210-ballot/ig/CodeSystem-TDDUIEncounterParticipant.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.1.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-03T09:45:25+00:00</t>
+    <t>2025-11-03T10:12:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>